<commit_message>
Bug fixes - Outlier detection
</commit_message>
<xml_diff>
--- a/AdjacencyMatrix.xlsx
+++ b/AdjacencyMatrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Github\AutoPart-ML-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A040BF2-9303-46EB-8201-94EB7C292E08}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FB50541-705D-4003-A505-DAB2ABAEDC35}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -340,23 +340,23 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E1">
         <v>1</v>
@@ -365,27 +365,27 @@
         <v>1</v>
       </c>
       <c r="G1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G2">
         <v>1</v>
@@ -393,16 +393,16 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -416,25 +416,25 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -442,22 +442,22 @@
         <v>1</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -465,19 +465,19 @@
         <v>1</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6">
         <v>0</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G6">
         <v>0</v>
@@ -485,7 +485,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -494,16 +494,16 @@
         <v>0</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F7">
         <v>0</v>
       </c>
       <c r="G7">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bug fixes for Outlier detection
</commit_message>
<xml_diff>
--- a/AdjacencyMatrix.xlsx
+++ b/AdjacencyMatrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Github\AutoPart-ML-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FB50541-705D-4003-A505-DAB2ABAEDC35}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E79C839-8C9A-418D-9669-8184B9F3BE29}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -337,23 +337,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>1</v>
       </c>
       <c r="B1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D1">
         <v>1</v>
@@ -362,15 +362,24 @@
         <v>1</v>
       </c>
       <c r="F1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="H1">
+        <v>1</v>
+      </c>
+      <c r="I1">
+        <v>0</v>
+      </c>
+      <c r="J1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -379,7 +388,7 @@
         <v>1</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -390,10 +399,19 @@
       <c r="G2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -413,13 +431,22 @@
       <c r="G3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -428,16 +455,25 @@
         <v>1</v>
       </c>
       <c r="E4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F4">
         <v>0</v>
       </c>
       <c r="G4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1</v>
       </c>
@@ -448,21 +484,30 @@
         <v>1</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5">
         <v>1</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -474,7 +519,7 @@
         <v>0</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6">
         <v>1</v>
@@ -482,10 +527,19 @@
       <c r="G6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -494,7 +548,7 @@
         <v>0</v>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -503,6 +557,111 @@
         <v>0</v>
       </c>
       <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>0</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>0</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10">
         <v>1</v>
       </c>
     </row>

</xml_diff>